<commit_message>
Add C to large-scale comparison
</commit_message>
<xml_diff>
--- a/Evaluation/Results.xlsx
+++ b/Evaluation/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>WASM</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>~34000</t>
+  </si>
+  <si>
+    <t>WebGPU 100000</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12712489063867016"/>
+          <c:y val="2.8070175438596492E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -188,6 +201,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$A$10:$D$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>83.026546583005654</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>94.676077957950952</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>126.6772688567285</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>120.89954507772144</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$A$11:$D$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>83.026546583005654</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>94.676077957950952</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>126.6772688567285</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>120.89954507772144</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$7:$D$7</c:f>
@@ -450,7 +523,457 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time for 10000</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> matrix multiplications (100x100 matrices)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$A$22:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>798.66572519421459</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>380.97918391024558</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>346.85960176032802</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$A$22:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>798.66572519421459</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>380.97918391024558</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>346.85960176032802</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$19:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>WASM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WebGPU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$20:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13605.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3286.92875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28937.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="606374696"/>
+        <c:axId val="606376264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="606374696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="606376264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="606376264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (milliseconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="606374696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -995,20 +1518,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1022,6 +2050,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1293,10 +2351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="L10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,9 +2508,45 @@
         <v>2.4832622451967761</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>_xlfn.STDEV.S(A2:A6)</f>
+        <v>83.026546583005654</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ref="B10:D11" si="2">_xlfn.STDEV.S(B2:B6)</f>
+        <v>94.676077957950952</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>126.6772688567285</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>120.89954507772144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>A10</f>
+        <v>83.026546583005654</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:D11" si="3">B10</f>
+        <v>94.676077957950952</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>126.6772688567285</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>120.89954507772144</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>100000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1462,19 +2556,116 @@
       <c r="B14" t="s">
         <v>1</v>
       </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13157.05</v>
+      </c>
       <c r="B15">
-        <v>4721.5</v>
+        <v>3192.1149999999998</v>
+      </c>
+      <c r="C15">
+        <v>29452</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14207.7</v>
+      </c>
       <c r="B16">
+        <v>3204.38</v>
+      </c>
+      <c r="C16">
+        <v>28787</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14346.93</v>
+      </c>
+      <c r="B17">
+        <v>2926.22</v>
+      </c>
+      <c r="C17">
+        <v>28696</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12711</v>
+      </c>
+      <c r="B18">
+        <v>3825</v>
+      </c>
+      <c r="C18">
+        <v>28814</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>AVERAGE(A15:A18)</f>
+        <v>13605.67</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(B15:B18)</f>
+        <v>3286.92875</v>
+      </c>
+      <c r="C20">
+        <f>AVERAGE(C15:C18)</f>
+        <v>28937.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>_xlfn.STDEV.S(A15:A18)</f>
+        <v>798.66572519421459</v>
+      </c>
+      <c r="B22">
+        <f>_xlfn.STDEV.S(B15:B18)</f>
+        <v>380.97918391024558</v>
+      </c>
+      <c r="C22">
+        <f>_xlfn.STDEV.S(C15:C18)</f>
+        <v>346.85960176032802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>4721.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25">
         <v>5282.75</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26">
         <v>4693.83</v>
       </c>
     </row>

</xml_diff>